<commit_message>
ButtonStyle Class, MainBackground Class 추가. MainFrame 배경사진및 GUI 컴포넌트 세부 수정
</commit_message>
<xml_diff>
--- a/WORKSPACE/Object_Project/ExcelSheet/db.xlsx
+++ b/WORKSPACE/Object_Project/ExcelSheet/db.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>사물함번호</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>sada</t>
+  </si>
+  <si>
+    <t>-204109293</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>-1715655579</t>
+  </si>
+  <si>
+    <t>asdasd</t>
   </si>
 </sst>
 </file>
@@ -95,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -152,6 +164,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
StartFrame, DataFrame, SearchFrame Class GUI 수정
</commit_message>
<xml_diff>
--- a/WORKSPACE/Object_Project/ExcelSheet/db.xlsx
+++ b/WORKSPACE/Object_Project/ExcelSheet/db.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="18">
   <si>
     <t>사물함번호</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>01012365789</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -181,6 +184,321 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6"/>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20"/>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21"/>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22"/>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23"/>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24"/>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25"/>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>